<commit_message>
QA [ Template changes, spell check  ] resolved
</commit_message>
<xml_diff>
--- a/public/media/gametemplate/GameTemplate.xlsx
+++ b/public/media/gametemplate/GameTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jithesh.k\Desktop\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jithesh.k\Desktop\PWC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07250DD1-2939-4D82-9F7D-E69B9652C612}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989E94EF-F845-4EF8-B85F-F88BC3A15258}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{7B608FAF-8BF9-43E7-9E4E-F0AE9CA28A9A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19008" windowHeight="8940" xr2:uid="{7B608FAF-8BF9-43E7-9E4E-F0AE9CA28A9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario" sheetId="2" r:id="rId1"/>
@@ -514,7 +514,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,7 +633,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -685,7 +685,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
@@ -751,7 +751,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>3</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>4</v>
@@ -797,7 +797,7 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>4</v>
@@ -817,7 +817,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>4</v>
@@ -831,7 +831,7 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>5</v>
@@ -863,7 +863,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>5</v>
@@ -883,7 +883,7 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>5</v>
@@ -897,7 +897,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>6</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="1">
         <v>6</v>
@@ -943,7 +943,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="1">
         <v>6</v>

</xml_diff>